<commit_message>
seperated file into two folders
</commit_message>
<xml_diff>
--- a/preprocessing/test.xlsx
+++ b/preprocessing/test.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\small\Desktop\VAMAP\Team16_Development\dataprocessing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\small\Desktop\VAMAP\Team16_Development\preprocessing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4C4C987-52BF-4D05-82F6-EDD5E8EB2D4C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD1A4C95-5F98-4CF9-91E7-8EBFE705247B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10932" xr2:uid="{D02863B5-8E0E-4777-9467-E13BE1258792}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10932" activeTab="1" xr2:uid="{D02863B5-8E0E-4777-9467-E13BE1258792}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="road" sheetId="1" r:id="rId1"/>
+    <sheet name="building" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="6">
   <si>
     <t>x</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -419,8 +420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9292E24D-DFD4-4470-9763-5C3B1C2D2351}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="A1:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -523,4 +524,113 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{260E8D69-6AF2-4B2F-8CD7-0D9ABF3F8DE5}">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A2">
+        <v>23</v>
+      </c>
+      <c r="B2">
+        <v>15.1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A3">
+        <v>14</v>
+      </c>
+      <c r="B3">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A4">
+        <v>24</v>
+      </c>
+      <c r="B4">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>